<commit_message>
Updated the changes after code review
</commit_message>
<xml_diff>
--- a/BenadrylAutomation/src/test/resources/TestData/AllergiesTestData.xlsx
+++ b/BenadrylAutomation/src/test/resources/TestData/AllergiesTestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SJI-GOA-69\git\BenadrylAutomation\BenadrylAutomation\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AE01A2E-C28C-46C0-9359-E2C3F44DA77C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{193BB6E1-9486-4C62-B089-80D35BCD36F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="allergiesNav" sheetId="1" r:id="rId1"/>
@@ -213,39 +213,6 @@
     <t>Allergy Symptoms and Common Causes of Allergic Reactions</t>
   </si>
   <si>
-    <t>Verify user is navigating to the  proper article "Are Allergies Causing Your Itchy, Sore Throat?" and asserting article name</t>
-  </si>
-  <si>
-    <t>Verify user is navigating to the  proper article "Tips And Remedies To Treat, Prevent, And Manage Allergy Symptoms" and asserting article name</t>
-  </si>
-  <si>
-    <t>Verify user is navigating to the  proper article "Dog &amp; Cat Allergies: How To Manage Pet Allergy Symptoms" and asserting article name</t>
-  </si>
-  <si>
-    <t>Verify user is navigating to the  proper article "Allergies At Night And How To Relieve Night Time Symptoms" and asserting article name</t>
-  </si>
-  <si>
-    <t>Verify user is navigating to the  proper article "Allergies On The Go: 10 Travel Tips For Allergy Prevention &amp; Relief" and asserting article name</t>
-  </si>
-  <si>
-    <t>Verify user is navigating to the  proper article "Outdoor Allergies Tips For Symptom Relief" and asserting article name</t>
-  </si>
-  <si>
-    <t>Verify user is navigating to the  proper article "Tips To Treat Nasal Congestion From Allergies At Home" and asserting article name</t>
-  </si>
-  <si>
-    <t>Verify user is navigating to the  proper article "Allergy Symptoms And Common Causes Of Allergic Reactions" and asserting article name</t>
-  </si>
-  <si>
-    <t>Verify user is navigating to the  proper article "Indoor Allergy Tips to Help Relieve Symptoms at Home" and asserting article name</t>
-  </si>
-  <si>
-    <t>Verify user is navigating to the  proper article "Ragweed Pollen Allergies: Symptoms, Treatment &amp; More" and asserting article name</t>
-  </si>
-  <si>
-    <t>Verify user is navigating to the  proper article "What Are Histamines &amp; How Do They Relate to Allergies?" and asserting article name</t>
-  </si>
-  <si>
     <t>Reference link</t>
   </si>
   <si>
@@ -400,51 +367,6 @@
   </si>
   <si>
     <t>Dye-Free Allergy</t>
-  </si>
-  <si>
-    <t>Verify user is navigated to peroper url after clicking on "histamine" link</t>
-  </si>
-  <si>
-    <t>Verify user is navigated to peroper url after clicking on "seasonal vs. year-round allergy guide" link</t>
-  </si>
-  <si>
-    <t>Verify user is navigated to peroper url after clicking on "ragweed" link</t>
-  </si>
-  <si>
-    <t>Verify user is navigated to peroper url after clicking on "allergy symptoms" link</t>
-  </si>
-  <si>
-    <t>Verify user is navigated to peroper url after clicking on "Congestion" link</t>
-  </si>
-  <si>
-    <t>Verify user is navigated to peroper url after clicking on "MORE ABOUT OUTDOOR ALLERGIES" link</t>
-  </si>
-  <si>
-    <t>Verify user is navigated to peroper url after clicking on "MORE ABOUT INDOOR ALLERGIES" link</t>
-  </si>
-  <si>
-    <t>Verify user is navigated to peroper url after clicking on "MORE ABOUT PET ALLERGIES" link</t>
-  </si>
-  <si>
-    <t>Verify user is navigated to peroper url after clicking on "LEARN IF IT IS A COLD OR ALLERGIES" link</t>
-  </si>
-  <si>
-    <t>Verify user is navigated to peroper url after clicking on "Allergy ULTRATABS" link</t>
-  </si>
-  <si>
-    <t>Verify user is navigated to peroper url after clicking on "Allergy LIQUI-GELS" link</t>
-  </si>
-  <si>
-    <t>Verify user is navigated to peroper url after clicking on "Allergy Plus Congestion" link</t>
-  </si>
-  <si>
-    <t>Verify user is navigated to peroper url after clicking on "Allergy Liquid" link</t>
-  </si>
-  <si>
-    <t>Verify user is navigated to peroper url after clicking on "Chewables" link</t>
-  </si>
-  <si>
-    <t>Verify user is navigated to peroper url after clicking on "Dye-Free Allergy" link</t>
   </si>
   <si>
     <t>Heading</t>
@@ -498,6 +420,84 @@
   </si>
   <si>
     <t>Benadryl Extra Strength Antihistamine Allergy Relief Tablets, 24 Count</t>
+  </si>
+  <si>
+    <t>Verify user is navigated to proper url after clicking on "histamine" link</t>
+  </si>
+  <si>
+    <t>Verify user is navigated to proper url after clicking on "seasonal vs. year-round allergy guide" link</t>
+  </si>
+  <si>
+    <t>Verify user is navigated to proper url after clicking on "ragweed" link</t>
+  </si>
+  <si>
+    <t>Verify user is navigated to proper url after clicking on "MORE ABOUT OUTDOOR ALLERGIES" link</t>
+  </si>
+  <si>
+    <t>Verify user is navigated to proper url after clicking on "MORE ABOUT INDOOR ALLERGIES" link</t>
+  </si>
+  <si>
+    <t>Verify user is navigated to proper url after clicking on "MORE ABOUT PET ALLERGIES" link</t>
+  </si>
+  <si>
+    <t>Verify user is navigated to proper url after clicking on "allergy symptoms" link</t>
+  </si>
+  <si>
+    <t>Verify user is navigated to proper url after clicking on "Congestion" link</t>
+  </si>
+  <si>
+    <t>Verify user is navigated to proper url after clicking on "LEARN IF IT IS A COLD OR ALLERGIES" link</t>
+  </si>
+  <si>
+    <t>Verify user is navigated to proper url after clicking on "Allergy ULTRATABS" link</t>
+  </si>
+  <si>
+    <t>Verify user is navigated to proper url after clicking on "Allergy LIQUI-GELS" link</t>
+  </si>
+  <si>
+    <t>Verify user is navigated to proper url after clicking on "Allergy Plus Congestion" link</t>
+  </si>
+  <si>
+    <t>Verify user is navigated to proper url after clicking on "Allergy Liquid" link</t>
+  </si>
+  <si>
+    <t>Verify user is navigated to proper url after clicking on "Chewables" link</t>
+  </si>
+  <si>
+    <t>Verify user is navigated to proper url after clicking on "Dye-Free Allergy" link</t>
+  </si>
+  <si>
+    <t>Verify user is navigating to the  proper article "Are Allergies Causing Your Itchy, Sore Throat?" and assert article name</t>
+  </si>
+  <si>
+    <t>Verify user is navigating to the  proper article "Tips And Remedies To Treat, Prevent, And Manage Allergy Symptoms" and assert article name</t>
+  </si>
+  <si>
+    <t>Verify user is navigating to the  proper article "Dog &amp; Cat Allergies: How To Manage Pet Allergy Symptoms" and assert article name</t>
+  </si>
+  <si>
+    <t>Verify user is navigating to the  proper article "Allergies At Night And How To Relieve Night Time Symptoms" and assert article name</t>
+  </si>
+  <si>
+    <t>Verify user is navigating to the  proper article "Allergies On The Go: 10 Travel Tips For Allergy Prevention &amp; Relief" and assert article name</t>
+  </si>
+  <si>
+    <t>Verify user is navigating to the  proper article "Outdoor Allergies Tips For Symptom Relief" and assert article name</t>
+  </si>
+  <si>
+    <t>Verify user is navigating to the  proper article "Tips To Treat Nasal Congestion From Allergies At Home" and assert article name</t>
+  </si>
+  <si>
+    <t>Verify user is navigating to the  proper article "Allergy Symptoms And Common Causes Of Allergic Reactions" and assert article name</t>
+  </si>
+  <si>
+    <t>Verify user is navigating to the  proper article "Indoor Allergy Tips to Help Relieve Symptoms at Home" and assert article name</t>
+  </si>
+  <si>
+    <t>Verify user is navigating to the  proper article "Ragweed Pollen Allergies: Symptoms, Treatment &amp; More" and assert article name</t>
+  </si>
+  <si>
+    <t>Verify user is navigating to the  proper article "What Are Histamines &amp; How Do They Relate to Allergies?" and assert article name</t>
   </si>
 </sst>
 </file>
@@ -1138,7 +1138,7 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D2"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1165,18 +1165,18 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
@@ -1191,15 +1191,15 @@
         <v>16</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
@@ -1214,15 +1214,15 @@
         <v>16</v>
       </c>
       <c r="F3" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="G3" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
@@ -1237,15 +1237,15 @@
         <v>17</v>
       </c>
       <c r="F4" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="G4" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
@@ -1260,15 +1260,15 @@
         <v>17</v>
       </c>
       <c r="F5" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="G5" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
@@ -1283,15 +1283,15 @@
         <v>18</v>
       </c>
       <c r="F6" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="G6" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
@@ -1306,15 +1306,15 @@
         <v>19</v>
       </c>
       <c r="F7" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="G7" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>126</v>
+        <v>135</v>
       </c>
       <c r="B8" t="s">
         <v>5</v>
@@ -1329,15 +1329,15 @@
         <v>20</v>
       </c>
       <c r="F8" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="G8" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
       <c r="B9" t="s">
         <v>5</v>
@@ -1352,15 +1352,15 @@
         <v>20</v>
       </c>
       <c r="F9" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="G9" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="B10" t="s">
         <v>5</v>
@@ -1375,15 +1375,15 @@
         <v>20</v>
       </c>
       <c r="F10" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="G10" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="B11" t="s">
         <v>5</v>
@@ -1398,15 +1398,15 @@
         <v>20</v>
       </c>
       <c r="F11" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="G11" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="B12" t="s">
         <v>5</v>
@@ -1421,15 +1421,15 @@
         <v>20</v>
       </c>
       <c r="F12" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="G12" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="B13" t="s">
         <v>5</v>
@@ -1444,15 +1444,15 @@
         <v>20</v>
       </c>
       <c r="F13" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="G13" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="B14" t="s">
         <v>5</v>
@@ -1467,15 +1467,15 @@
         <v>20</v>
       </c>
       <c r="F14" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="G14" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="B15" t="s">
         <v>5</v>
@@ -1490,15 +1490,15 @@
         <v>20</v>
       </c>
       <c r="F15" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="G15" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="B16" t="s">
         <v>5</v>
@@ -1513,15 +1513,15 @@
         <v>20</v>
       </c>
       <c r="F16" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="G16" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="B17" t="s">
         <v>5</v>
@@ -1536,10 +1536,10 @@
         <v>20</v>
       </c>
       <c r="F17" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="G17" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -1551,7 +1551,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6E5A3EC-BB8B-4F38-A0B6-037F14E75CB3}">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1585,7 +1587,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>60</v>
+        <v>144</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
@@ -1605,7 +1607,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>61</v>
+        <v>145</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
@@ -1625,7 +1627,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>62</v>
+        <v>146</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
@@ -1645,7 +1647,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>63</v>
+        <v>147</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
@@ -1665,7 +1667,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>64</v>
+        <v>148</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
@@ -1685,7 +1687,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>65</v>
+        <v>149</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
@@ -1705,7 +1707,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>66</v>
+        <v>150</v>
       </c>
       <c r="B8" t="s">
         <v>5</v>
@@ -1725,7 +1727,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>67</v>
+        <v>151</v>
       </c>
       <c r="B9" t="s">
         <v>5</v>
@@ -1745,7 +1747,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>68</v>
+        <v>152</v>
       </c>
       <c r="B10" t="s">
         <v>5</v>
@@ -1765,7 +1767,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>69</v>
+        <v>153</v>
       </c>
       <c r="B11" t="s">
         <v>5</v>
@@ -1785,7 +1787,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>70</v>
+        <v>154</v>
       </c>
       <c r="B12" t="s">
         <v>5</v>
@@ -1812,7 +1814,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{121339D2-9F26-4974-9A0D-2FEABAB69C14}">
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
@@ -1841,24 +1843,24 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>138</v>
+        <v>112</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>139</v>
+        <v>113</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>140</v>
+        <v>114</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>141</v>
+        <v>115</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>142</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>149</v>
+        <v>123</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>5</v>
@@ -1873,21 +1875,21 @@
         <v>39</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>147</v>
+        <v>121</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>144</v>
+        <v>118</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>148</v>
+        <v>122</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>150</v>
+        <v>124</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>5</v>
@@ -1902,21 +1904,21 @@
         <v>39</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>143</v>
+        <v>117</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>144</v>
+        <v>118</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>145</v>
+        <v>119</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>151</v>
+        <v>125</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>5</v>
@@ -1931,16 +1933,16 @@
         <v>39</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>152</v>
+        <v>126</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>153</v>
+        <v>127</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>146</v>
+        <v>120</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>154</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -1980,15 +1982,15 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>5</v>
@@ -2000,15 +2002,15 @@
         <v>7</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>5</v>
@@ -2020,15 +2022,15 @@
         <v>7</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>5</v>
@@ -2040,15 +2042,15 @@
         <v>7</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>5</v>
@@ -2060,15 +2062,15 @@
         <v>7</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>5</v>
@@ -2080,15 +2082,15 @@
         <v>7</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>5</v>
@@ -2100,10 +2102,10 @@
         <v>7</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Committed after code review
</commit_message>
<xml_diff>
--- a/BenadrylAutomation/src/test/resources/TestData/AllergiesTestData.xlsx
+++ b/BenadrylAutomation/src/test/resources/TestData/AllergiesTestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SJI-GOA-69\git\BenadrylAutomation\BenadrylAutomation\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{193BB6E1-9486-4C62-B089-80D35BCD36F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C52529A9-76AE-442D-9E35-990CD8681D8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="allergiesNav" sheetId="1" r:id="rId1"/>
@@ -255,24 +255,6 @@
     <t>https://www.mayoclinic.org/diseases-conditions/common-cold/expert-answers/common-cold/faq-20057857</t>
   </si>
   <si>
-    <t>Verify user is navigating to the proper references "Cleveland Clinic. Allergy Overview." and asserting url</t>
-  </si>
-  <si>
-    <t>Verify user is navigating to the proper references "Mayo Clinic. Cold or allergy" and asserting url</t>
-  </si>
-  <si>
-    <t>Verify user is navigating to the proper references "American College of Allergy, Asthma, &amp; Immunology." and asserting url</t>
-  </si>
-  <si>
-    <t>Verify user is navigating to the proper references "Asthma and Allergy Foundation of America. Pet Allergy" and asserting url</t>
-  </si>
-  <si>
-    <t>Verify user is navigating to the proper references "Asthma and Allergy Foundation of America. Pollen Allergy." and asserting url</t>
-  </si>
-  <si>
-    <t>Verify user is navigating to the proper references "American College of Allergy, Asthma, &amp; Immunology. Allergy Symptoms." and asserting url</t>
-  </si>
-  <si>
     <t>jumpToName</t>
   </si>
   <si>
@@ -498,6 +480,24 @@
   </si>
   <si>
     <t>Verify user is navigating to the  proper article "What Are Histamines &amp; How Do They Relate to Allergies?" and assert article name</t>
+  </si>
+  <si>
+    <t>Verify reference "Cleveland Clinic. Allergy Overview."</t>
+  </si>
+  <si>
+    <t>Verify reference "American College of Allergy, Asthma, &amp; Immunology. Allergy Symptoms."</t>
+  </si>
+  <si>
+    <t>Verify reference "Asthma and Allergy Foundation of America. Pollen Allergy."</t>
+  </si>
+  <si>
+    <t>Verify reference "Asthma and Allergy Foundation of America. Pet Allergy"</t>
+  </si>
+  <si>
+    <t>Verify reference "American College of Allergy, Asthma, &amp; Immunology."</t>
+  </si>
+  <si>
+    <t>Verify reference "Mayo Clinic. Cold or allergy"</t>
   </si>
 </sst>
 </file>
@@ -1165,18 +1165,18 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
@@ -1191,15 +1191,15 @@
         <v>16</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
@@ -1214,15 +1214,15 @@
         <v>16</v>
       </c>
       <c r="F3" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="G3" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
@@ -1237,15 +1237,15 @@
         <v>17</v>
       </c>
       <c r="F4" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="G4" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
@@ -1260,15 +1260,15 @@
         <v>17</v>
       </c>
       <c r="F5" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="G5" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
@@ -1283,15 +1283,15 @@
         <v>18</v>
       </c>
       <c r="F6" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="G6" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
@@ -1306,15 +1306,15 @@
         <v>19</v>
       </c>
       <c r="F7" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="G7" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="B8" t="s">
         <v>5</v>
@@ -1329,15 +1329,15 @@
         <v>20</v>
       </c>
       <c r="F8" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="G8" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="B9" t="s">
         <v>5</v>
@@ -1352,15 +1352,15 @@
         <v>20</v>
       </c>
       <c r="F9" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="G9" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="B10" t="s">
         <v>5</v>
@@ -1375,15 +1375,15 @@
         <v>20</v>
       </c>
       <c r="F10" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="G10" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="B11" t="s">
         <v>5</v>
@@ -1398,15 +1398,15 @@
         <v>20</v>
       </c>
       <c r="F11" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="G11" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="B12" t="s">
         <v>5</v>
@@ -1421,15 +1421,15 @@
         <v>20</v>
       </c>
       <c r="F12" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="G12" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="B13" t="s">
         <v>5</v>
@@ -1444,15 +1444,15 @@
         <v>20</v>
       </c>
       <c r="F13" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="G13" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="B14" t="s">
         <v>5</v>
@@ -1467,15 +1467,15 @@
         <v>20</v>
       </c>
       <c r="F14" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="G14" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="B15" t="s">
         <v>5</v>
@@ -1490,15 +1490,15 @@
         <v>20</v>
       </c>
       <c r="F15" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="G15" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="B16" t="s">
         <v>5</v>
@@ -1513,15 +1513,15 @@
         <v>20</v>
       </c>
       <c r="F16" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="G16" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="B17" t="s">
         <v>5</v>
@@ -1536,10 +1536,10 @@
         <v>20</v>
       </c>
       <c r="F17" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="G17" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -1551,7 +1551,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6E5A3EC-BB8B-4F38-A0B6-037F14E75CB3}">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
@@ -1587,7 +1587,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
@@ -1607,7 +1607,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
@@ -1627,7 +1627,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
@@ -1647,7 +1647,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
@@ -1667,7 +1667,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
@@ -1687,7 +1687,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
@@ -1707,7 +1707,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="B8" t="s">
         <v>5</v>
@@ -1727,7 +1727,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="B9" t="s">
         <v>5</v>
@@ -1747,7 +1747,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="B10" t="s">
         <v>5</v>
@@ -1767,7 +1767,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="B11" t="s">
         <v>5</v>
@@ -1787,7 +1787,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="B12" t="s">
         <v>5</v>
@@ -1843,24 +1843,24 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>5</v>
@@ -1875,21 +1875,21 @@
         <v>39</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>5</v>
@@ -1904,21 +1904,21 @@
         <v>39</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>5</v>
@@ -1933,16 +1933,16 @@
         <v>39</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>
@@ -1954,13 +1954,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9ADF491-2C10-49FE-821F-533EAD642EE7}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A7"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="71.44140625" customWidth="1"/>
+    <col min="1" max="1" width="70.109375" customWidth="1"/>
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
@@ -1988,9 +1986,9 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>74</v>
+        <v>149</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>5</v>
@@ -2008,9 +2006,9 @@
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>79</v>
+        <v>150</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>5</v>
@@ -2030,7 +2028,7 @@
     </row>
     <row r="4" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>78</v>
+        <v>151</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>5</v>
@@ -2050,7 +2048,7 @@
     </row>
     <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>77</v>
+        <v>152</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>5</v>
@@ -2068,9 +2066,9 @@
         <v>71</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>76</v>
+        <v>153</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>5</v>
@@ -2090,7 +2088,7 @@
     </row>
     <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>75</v>
+        <v>154</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>5</v>

</xml_diff>